<commit_message>
Wrote 6.3 (MRR Recall Precision)
</commit_message>
<xml_diff>
--- a/paper/resource/cross_validation_file_63percommit_mrr_cost.xlsx
+++ b/paper/resource/cross_validation_file_63percommit_mrr_cost.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26518"/>
   <workbookPr date1904="1" showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14280" yWindow="2900" windowWidth="25360" windowHeight="15820" tabRatio="895" activeTab="6"/>
+    <workbookView xWindow="4100" yWindow="4980" windowWidth="25360" windowHeight="15820" tabRatio="895" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="minconf_table.csv" sheetId="1" r:id="rId1"/>
@@ -79,10 +79,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>precision</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>recall</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -118,14 +114,17 @@
     <t>Co-chg rules (minsup=0.006)</t>
     <phoneticPr fontId="2"/>
   </si>
+  <si>
+    <t>MRR</t>
+    <phoneticPr fontId="2"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.0000%"/>
-    <numFmt numFmtId="177" formatCode="0.000%"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -187,7 +186,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="454">
+  <cellStyleXfs count="502">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -642,15 +641,62 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="437" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="437" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="437" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="454">
+  <cellStyles count="502">
     <cellStyle name="パーセント" xfId="437" builtinId="5"/>
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
@@ -878,6 +924,30 @@
     <cellStyle name="ハイパーリンク" xfId="448" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="450" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="452" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="454" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="456" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="458" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="460" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="462" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="464" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="466" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="468" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="470" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="472" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="474" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="476" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="478" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="480" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="482" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="484" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="486" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="488" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="490" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="492" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="494" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="496" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="498" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="500" builtinId="8" hidden="1"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="4" builtinId="9" hidden="1"/>
@@ -1105,8 +1175,192 @@
     <cellStyle name="表示済みのハイパーリンク" xfId="449" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="451" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="453" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="455" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="457" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="459" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="461" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="463" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="465" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="467" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="469" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="471" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="473" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="475" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="477" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="479" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="481" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="483" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="485" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="487" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="489" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="491" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="493" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="495" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="497" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="499" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="501" builtinId="9" hidden="1"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="20">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1184,9 +1438,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.150100974639317"/>
-          <c:y val="0.0339561043241688"/>
+          <c:y val="0.369372703412073"/>
           <c:w val="0.787936205426551"/>
-          <c:h val="0.827245884037223"/>
+          <c:h val="0.491829232283464"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1859,11 +2113,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2138583080"/>
-        <c:axId val="2117251080"/>
+        <c:axId val="2063121224"/>
+        <c:axId val="-2100881224"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2138583080"/>
+        <c:axId val="2063121224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1931,7 +2185,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2117251080"/>
+        <c:crossAx val="-2100881224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1939,7 +2193,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2117251080"/>
+        <c:axId val="-2100881224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1987,7 +2241,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2138583080"/>
+        <c:crossAx val="2063121224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2001,6 +2255,37 @@
         </a:ln>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.183264844040418"/>
+          <c:y val="0.0166666666666667"/>
+          <c:w val="0.627032543678821"/>
+          <c:h val="0.321351541994751"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800"/>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -2407,11 +2692,522 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2128407192"/>
-        <c:axId val="2118576888"/>
+        <c:axId val="-2127037944"/>
+        <c:axId val="-2099565112"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2128407192"/>
+        <c:axId val="-2127037944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                  <a:lnSpc>
+                    <a:spcPct val="100000"/>
+                  </a:lnSpc>
+                  <a:spcBef>
+                    <a:spcPts val="0"/>
+                  </a:spcBef>
+                  <a:spcAft>
+                    <a:spcPts val="0"/>
+                  </a:spcAft>
+                  <a:buClrTx/>
+                  <a:buSzTx/>
+                  <a:buFontTx/>
+                  <a:buNone/>
+                  <a:tabLst/>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="ja-JP"/>
+                  <a:t>minimum confidence</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2099565112"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2099565112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="ja-JP"/>
+                  <a:t>precision</a:t>
+                </a:r>
+                <a:endParaRPr lang="ja-JP" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2127037944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="0.2"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="ja-JP"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>recall!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Co-ref rules (minsup=0.002)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>recall!$B$1:$J$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>recall!$B$2:$J$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.331719038798804</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.283549637669567</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.26288996153016</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.229548793390029</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.200710241307971</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.169390803595883</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.117757660989947</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.108788258334117</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0997182424035591</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>recall!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Co-chg rules (minsup=0.002)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>recall!$B$1:$J$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>recall!$B$3:$J$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.223686243432691</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.186541009168176</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.145963421902291</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.11207207806792</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.083968060263149</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.063567346412174</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0424772113344513</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0332594874312331</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0224832215286103</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>recall!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Co-ref rules (minsup=0.004)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>recall!$B$1:$J$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>recall!$B$4:$J$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.262734525766234</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.211947102105567</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.190578498622429</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.154681873798076</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.12850364385371</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0966670059809921</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0711687142945231</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0551398112244106</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0423672237533763</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>recall!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Co-chg rules (minsup=0.004)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>recall!$B$1:$J$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>recall!$B$5:$J$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.109658673073495</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.083088084036584</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0555081535281284</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0353811858514611</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.021938578291768</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0111904418011001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.00582393151362623</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.00273895555804035</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.000572733194837176</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2134207720"/>
+        <c:axId val="-2099291752"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2134207720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2460,7 +3256,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2118576888"/>
+        <c:crossAx val="-2099291752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2468,515 +3264,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2118576888"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="1.0"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" vert="horz"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" altLang="ja-JP"/>
-                  <a:t>precision</a:t>
-                </a:r>
-                <a:endParaRPr lang="ja-JP" altLang="en-US"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2128407192"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-        <c:majorUnit val="0.2"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="1"/>
-  <c:lang val="ja-JP"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>recall!$A$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Co-ref rules (minsup=0.002)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>recall!$B$1:$J$1</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.9</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>recall!$B$2:$J$2</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>0.331719038798804</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.283549637669567</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.26288996153016</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.229548793390029</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.200710241307971</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.169390803595883</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.117757660989947</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.108788258334117</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.0997182424035591</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>recall!$A$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Co-chg rules (minsup=0.002)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>recall!$B$1:$J$1</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.9</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>recall!$B$3:$J$3</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>0.223686243432691</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.186541009168176</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.145963421902291</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.11207207806792</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.083968060263149</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.063567346412174</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.0424772113344513</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.0332594874312331</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.0224832215286103</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>recall!$A$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Co-ref rules (minsup=0.004)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>recall!$B$1:$J$1</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.9</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>recall!$B$4:$J$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>0.262734525766234</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.211947102105567</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.190578498622429</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.154681873798076</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.12850364385371</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.0966670059809921</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.0711687142945231</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.0551398112244106</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.0423672237533763</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>recall!$A$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Co-chg rules (minsup=0.004)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>recall!$B$1:$J$1</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.9</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>recall!$B$5:$J$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>0.109658673073495</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.083088084036584</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.0555081535281284</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.0353811858514611</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.021938578291768</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.0111904418011001</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.00582393151362623</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.00273895555804035</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.000572733194837176</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="2138302280"/>
-        <c:axId val="2117282024"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="2138302280"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-                  <a:lnSpc>
-                    <a:spcPct val="100000"/>
-                  </a:lnSpc>
-                  <a:spcBef>
-                    <a:spcPts val="0"/>
-                  </a:spcBef>
-                  <a:spcAft>
-                    <a:spcPts val="0"/>
-                  </a:spcAft>
-                  <a:buClrTx/>
-                  <a:buSzTx/>
-                  <a:buFontTx/>
-                  <a:buNone/>
-                  <a:tabLst/>
-                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:sysClr val="windowText" lastClr="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" altLang="ja-JP"/>
-                  <a:t>minimum confidence</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2117282024"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="2117282024"/>
+        <c:axId val="-2099291752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -3007,7 +3295,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2138302280"/>
+        <c:crossAx val="-2134207720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -4272,11 +4560,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2117793816"/>
-        <c:axId val="2138728168"/>
+        <c:axId val="-2068029032"/>
+        <c:axId val="-2068664200"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2117793816"/>
+        <c:axId val="-2068029032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -4324,13 +4612,13 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2138728168"/>
+        <c:crossAx val="-2068664200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2138728168"/>
+        <c:axId val="-2068664200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.5"/>
@@ -4349,7 +4637,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" altLang="ja-JP" sz="1800"/>
-                  <a:t>Precision</a:t>
+                  <a:t>MRR</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -4371,7 +4659,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2117793816"/>
+        <c:crossAx val="-2068029032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -4704,6 +4992,7 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -4948,6 +5237,7 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="8"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -5491,6 +5781,7 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -5539,6 +5830,7 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="8"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -5647,11 +5939,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2128844792"/>
-        <c:axId val="-2077318312"/>
+        <c:axId val="-2068281432"/>
+        <c:axId val="-2053334824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2128844792"/>
+        <c:axId val="-2068281432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -5699,13 +5991,13 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2077318312"/>
+        <c:crossAx val="-2053334824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2077318312"/>
+        <c:axId val="-2053334824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -5729,6 +6021,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -5745,7 +6038,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2128844792"/>
+        <c:crossAx val="-2068281432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -5819,9 +6112,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.173676931803016"/>
-          <c:y val="0.0615529063080598"/>
-          <c:w val="0.774099326037635"/>
-          <c:h val="0.80807860744935"/>
+          <c:y val="0.316963340647993"/>
+          <c:w val="0.778283365729911"/>
+          <c:h val="0.55266825868078"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -6498,11 +6791,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2073551896"/>
-        <c:axId val="-2074033432"/>
+        <c:axId val="-2053493304"/>
+        <c:axId val="-2068416552"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2073551896"/>
+        <c:axId val="-2053493304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6525,6 +6818,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -6541,7 +6835,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2074033432"/>
+        <c:crossAx val="-2068416552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6549,7 +6843,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2074033432"/>
+        <c:axId val="-2068416552"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -6579,6 +6873,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.E+00" sourceLinked="0"/>
@@ -6595,7 +6890,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2073551896"/>
+        <c:crossAx val="-2053493304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6609,6 +6904,41 @@
         </a:ln>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.253321716831325"/>
+          <c:y val="0.0245521304517786"/>
+          <c:w val="0.594569264647004"/>
+          <c:h val="0.264743068253909"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -6627,12 +6957,12 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
+      <xdr:colOff>622300</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>215900</xdr:rowOff>
     </xdr:to>
@@ -6810,14 +7140,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>850900</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>215900</xdr:rowOff>
     </xdr:to>
@@ -7169,7 +7499,7 @@
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34:J37"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -7208,7 +7538,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -7373,7 +7703,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -7538,7 +7868,7 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -7703,7 +8033,7 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -7868,7 +8198,7 @@
     </row>
     <row r="26" spans="1:10">
       <c r="A26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -8033,7 +8363,7 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -8213,8 +8543,8 @@
   <sheetPr codeName="Sheet10" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -8227,13 +8557,13 @@
         <v>12</v>
       </c>
       <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
         <v>13</v>
-      </c>
-      <c r="C1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -8241,13 +8571,13 @@
         <v>2E-3</v>
       </c>
       <c r="B2" s="3">
-        <v>0.5</v>
+        <v>1.222E-2</v>
       </c>
       <c r="C2" s="3">
+        <v>0.9748</v>
+      </c>
+      <c r="D2" s="3">
         <v>9.3790000000000002E-3</v>
-      </c>
-      <c r="D2" s="3">
-        <v>6.1700000000000004E-4</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -8255,13 +8585,13 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="B3" s="3">
-        <v>0.56830000000000003</v>
+        <v>6.1700000000000004E-4</v>
       </c>
       <c r="C3" s="3">
+        <v>0.129</v>
+      </c>
+      <c r="D3" s="3">
         <v>1.9949999999999998E-3</v>
-      </c>
-      <c r="D3" s="4">
-        <v>2.0570000000000001E-5</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -8269,18 +8599,18 @@
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="B4" s="3">
-        <v>0.25919999999999999</v>
+        <v>9.4909999999999994E-3</v>
       </c>
       <c r="C4" s="3">
+        <v>2.997E-2</v>
+      </c>
+      <c r="D4" s="3">
         <v>1.4489999999999999E-2</v>
-      </c>
-      <c r="D4" s="3">
-        <v>3.4970000000000001E-3</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -8288,6 +8618,11 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>
+  <conditionalFormatting sqref="B2:D4">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+      <formula>0.025</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -9316,7 +9651,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="J2" sqref="B2:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -9618,16 +9953,16 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="B2:J2">
-    <cfRule type="top10" dxfId="3" priority="4" rank="1"/>
+    <cfRule type="top10" dxfId="13" priority="4" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:J3">
-    <cfRule type="top10" dxfId="2" priority="3" rank="1"/>
+    <cfRule type="top10" dxfId="12" priority="3" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:J4">
-    <cfRule type="top10" dxfId="1" priority="2" rank="1"/>
+    <cfRule type="top10" dxfId="11" priority="2" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:J5">
-    <cfRule type="top10" dxfId="0" priority="1" rank="1"/>
+    <cfRule type="top10" dxfId="10" priority="1" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -9646,7 +9981,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -9947,6 +10282,24 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>
+  <conditionalFormatting sqref="B2:J2">
+    <cfRule type="top10" dxfId="9" priority="6" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3:J3">
+    <cfRule type="top10" dxfId="8" priority="5" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:J4">
+    <cfRule type="top10" dxfId="6" priority="4" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5:J5">
+    <cfRule type="top10" dxfId="5" priority="3" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6:J6">
+    <cfRule type="top10" dxfId="4" priority="2" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7:J7">
+    <cfRule type="top10" dxfId="3" priority="1" rank="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
@@ -10597,8 +10950,8 @@
   <sheetPr codeName="Sheet8" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -11742,8 +12095,8 @@
   <sheetPr codeName="Sheet9" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>

</xml_diff>